<commit_message>
check of find of row(for type-eq)
</commit_message>
<xml_diff>
--- a/eq.xlsx
+++ b/eq.xlsx
@@ -7,12 +7,9 @@
     <workbookView xWindow="0" yWindow="30" windowWidth="22980" windowHeight="9795"/>
   </bookViews>
   <sheets>
-    <sheet name="eq" sheetId="2" r:id="rId1"/>
+    <sheet name="eq1" sheetId="2" r:id="rId1"/>
     <sheet name="applicator" sheetId="3" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">eq!$A$1:$K$94</definedName>
-  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -31,7 +28,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>1 для пістолетів
 3 для контролерів</t>
@@ -539,7 +537,8 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -879,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:K94"/>
+  <dimension ref="B1:K93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -895,13 +894,37 @@
     <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:11">
+      <c r="B1">
+        <v>80000025</v>
+      </c>
+      <c r="C1">
+        <f t="shared" ref="C1:C32" si="0">B1-80000000</f>
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="2" spans="2:11">
       <c r="B2">
-        <v>80000025</v>
+        <v>80000026</v>
       </c>
       <c r="C2">
-        <f>B2-80000000</f>
-        <v>25</v>
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -916,70 +939,70 @@
         <v>40</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="2:11">
       <c r="B3">
-        <v>80000026</v>
+        <v>80000046</v>
       </c>
       <c r="C3">
-        <f>B3-80000000</f>
-        <v>26</v>
+        <f t="shared" si="0"/>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>67</v>
       </c>
       <c r="I3" t="s">
-        <v>47</v>
+        <v>68</v>
+      </c>
+      <c r="J3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="2:11">
       <c r="B4">
-        <v>80000046</v>
+        <v>80000065</v>
       </c>
       <c r="C4">
-        <f>B4-80000000</f>
-        <v>46</v>
+        <f t="shared" si="0"/>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="E4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>113</v>
       </c>
       <c r="G4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="I4" t="s">
-        <v>68</v>
-      </c>
-      <c r="J4" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="2:11">
       <c r="B5">
-        <v>80000065</v>
+        <v>80000066</v>
       </c>
       <c r="C5">
-        <f>B5-80000000</f>
-        <v>65</v>
+        <f t="shared" si="0"/>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
         <v>101</v>
@@ -993,17 +1016,14 @@
       <c r="G5" t="s">
         <v>114</v>
       </c>
-      <c r="I5" t="s">
-        <v>116</v>
-      </c>
     </row>
     <row r="6" spans="2:11">
       <c r="B6">
-        <v>80000066</v>
+        <v>80000067</v>
       </c>
       <c r="C6">
-        <f>B6-80000000</f>
-        <v>66</v>
+        <f t="shared" si="0"/>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
         <v>101</v>
@@ -1017,221 +1037,224 @@
       <c r="G6" t="s">
         <v>114</v>
       </c>
+      <c r="I6" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="7" spans="2:11">
       <c r="B7">
-        <v>80000067</v>
+        <v>80000117</v>
       </c>
       <c r="C7">
-        <f>B7-80000000</f>
-        <v>67</v>
+        <f t="shared" si="0"/>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F7" t="s">
-        <v>113</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>114</v>
-      </c>
-      <c r="I7" t="s">
-        <v>115</v>
+        <v>45</v>
+      </c>
+      <c r="I7">
+        <v>891</v>
       </c>
     </row>
     <row r="8" spans="2:11">
       <c r="B8">
-        <v>80000117</v>
+        <v>80000123</v>
       </c>
       <c r="C8">
-        <f>B8-80000000</f>
+        <f t="shared" si="0"/>
+        <v>123</v>
+      </c>
+      <c r="D8" t="s">
         <v>117</v>
       </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
       <c r="E8" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>123</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8">
-        <v>891</v>
+        <v>124</v>
+      </c>
+      <c r="I8" t="s">
+        <v>132</v>
+      </c>
+      <c r="K8" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="2:11">
       <c r="B9">
-        <v>80000123</v>
+        <v>80000186</v>
       </c>
       <c r="C9">
-        <f>B9-80000000</f>
-        <v>123</v>
+        <f t="shared" si="0"/>
+        <v>186</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>124</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>123</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="I9" t="s">
-        <v>132</v>
-      </c>
-      <c r="K9" t="s">
-        <v>133</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:11">
       <c r="B10">
-        <v>80000186</v>
+        <v>80000287</v>
       </c>
       <c r="C10">
-        <f>B10-80000000</f>
-        <v>186</v>
+        <f t="shared" si="0"/>
+        <v>287</v>
       </c>
       <c r="D10" t="s">
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>122</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>129</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="I10" t="s">
-        <v>43</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="2:11">
       <c r="B11">
-        <v>80000287</v>
+        <v>80000307</v>
       </c>
       <c r="C11">
-        <f>B11-80000000</f>
-        <v>287</v>
+        <f t="shared" si="0"/>
+        <v>307</v>
       </c>
       <c r="D11" t="s">
-        <v>117</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>122</v>
+        <v>62</v>
       </c>
       <c r="F11" t="s">
-        <v>129</v>
+        <v>63</v>
       </c>
       <c r="G11" t="s">
-        <v>130</v>
-      </c>
-      <c r="I11" t="s">
-        <v>131</v>
+        <v>64</v>
+      </c>
+      <c r="I11">
+        <v>80703</v>
+      </c>
+      <c r="K11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="2:11">
       <c r="B12">
-        <v>80000307</v>
+        <v>80001214</v>
       </c>
       <c r="C12">
-        <f>B12-80000000</f>
-        <v>307</v>
+        <f t="shared" si="0"/>
+        <v>1214</v>
       </c>
       <c r="D12" t="s">
         <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>60</v>
+      </c>
+      <c r="H12" t="s">
+        <v>61</v>
       </c>
       <c r="I12">
-        <v>80703</v>
-      </c>
-      <c r="K12" t="s">
-        <v>65</v>
+        <v>544979</v>
+      </c>
+      <c r="J12">
+        <v>11390</v>
       </c>
     </row>
     <row r="13" spans="2:11">
       <c r="B13">
-        <v>80001214</v>
+        <v>80001235</v>
       </c>
       <c r="C13">
-        <f>B13-80000000</f>
-        <v>1214</v>
+        <f t="shared" si="0"/>
+        <v>1235</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>158</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" t="s">
-        <v>61</v>
+        <v>9</v>
+      </c>
+      <c r="H13">
+        <v>52960</v>
       </c>
       <c r="I13">
-        <v>544979</v>
-      </c>
-      <c r="J13">
-        <v>11390</v>
+        <v>333.29559999999998</v>
       </c>
     </row>
     <row r="14" spans="2:11">
       <c r="B14">
-        <v>80001235</v>
+        <v>80001236</v>
       </c>
       <c r="C14">
-        <f>B14-80000000</f>
-        <v>1235</v>
+        <f t="shared" si="0"/>
+        <v>1236</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="E14" t="s">
-        <v>158</v>
+        <v>77</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="G14" t="s">
         <v>9</v>
       </c>
-      <c r="H14">
-        <v>52960</v>
-      </c>
       <c r="I14">
-        <v>333.29559999999998</v>
+        <v>721.24850000000004</v>
       </c>
     </row>
     <row r="15" spans="2:11">
       <c r="B15">
-        <v>80001236</v>
+        <v>80001237</v>
       </c>
       <c r="C15">
-        <f>B15-80000000</f>
-        <v>1236</v>
+        <f t="shared" si="0"/>
+        <v>1237</v>
       </c>
       <c r="D15" t="s">
         <v>70</v>
@@ -1246,16 +1269,16 @@
         <v>9</v>
       </c>
       <c r="I15">
-        <v>721.24850000000004</v>
+        <v>721.24860000000001</v>
       </c>
     </row>
     <row r="16" spans="2:11">
       <c r="B16">
-        <v>80001237</v>
+        <v>80001238</v>
       </c>
       <c r="C16">
-        <f>B16-80000000</f>
-        <v>1237</v>
+        <f t="shared" si="0"/>
+        <v>1238</v>
       </c>
       <c r="D16" t="s">
         <v>70</v>
@@ -1270,88 +1293,91 @@
         <v>9</v>
       </c>
       <c r="I16">
-        <v>721.24860000000001</v>
+        <v>721.24869999999999</v>
       </c>
     </row>
     <row r="17" spans="2:11">
       <c r="B17">
-        <v>80001238</v>
+        <v>80001639</v>
       </c>
       <c r="C17">
-        <f>B17-80000000</f>
-        <v>1238</v>
+        <f t="shared" si="0"/>
+        <v>1639</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="F17" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="G17" t="s">
-        <v>9</v>
-      </c>
-      <c r="I17">
-        <v>721.24869999999999</v>
+        <v>56</v>
+      </c>
+      <c r="K17" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="2:11">
       <c r="B18">
-        <v>80001639</v>
+        <v>80001690</v>
       </c>
       <c r="C18">
-        <f>B18-80000000</f>
-        <v>1639</v>
+        <f t="shared" si="0"/>
+        <v>1690</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>117</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>123</v>
       </c>
       <c r="G18" t="s">
-        <v>56</v>
-      </c>
-      <c r="K18" t="s">
-        <v>57</v>
+        <v>127</v>
+      </c>
+      <c r="I18" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="2:11">
       <c r="B19">
-        <v>80001690</v>
+        <v>80001720</v>
       </c>
       <c r="C19">
-        <f>B19-80000000</f>
-        <v>1690</v>
+        <f t="shared" si="0"/>
+        <v>1720</v>
       </c>
       <c r="D19" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="E19" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
       <c r="F19" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="G19" t="s">
-        <v>127</v>
-      </c>
-      <c r="I19" t="s">
-        <v>128</v>
+        <v>9</v>
+      </c>
+      <c r="H19" t="s">
+        <v>95</v>
+      </c>
+      <c r="I19">
+        <v>16502</v>
       </c>
     </row>
     <row r="20" spans="2:11">
       <c r="B20">
-        <v>80001720</v>
+        <v>80001721</v>
       </c>
       <c r="C20">
-        <f>B20-80000000</f>
-        <v>1720</v>
+        <f t="shared" si="0"/>
+        <v>1721</v>
       </c>
       <c r="D20" t="s">
         <v>70</v>
@@ -1360,25 +1386,25 @@
         <v>73</v>
       </c>
       <c r="F20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G20" t="s">
         <v>9</v>
       </c>
       <c r="H20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I20">
-        <v>16502</v>
+        <v>16151</v>
       </c>
     </row>
     <row r="21" spans="2:11">
       <c r="B21">
-        <v>80001721</v>
+        <v>80001722</v>
       </c>
       <c r="C21">
-        <f>B21-80000000</f>
-        <v>1721</v>
+        <f t="shared" si="0"/>
+        <v>1722</v>
       </c>
       <c r="D21" t="s">
         <v>70</v>
@@ -1387,25 +1413,25 @@
         <v>73</v>
       </c>
       <c r="F21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G21" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" t="s">
-        <v>93</v>
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>45831</v>
       </c>
       <c r="I21">
-        <v>16151</v>
+        <v>761.3895</v>
       </c>
     </row>
     <row r="22" spans="2:11">
       <c r="B22">
-        <v>80001722</v>
+        <v>80001723</v>
       </c>
       <c r="C22">
-        <f>B22-80000000</f>
-        <v>1722</v>
+        <f t="shared" si="0"/>
+        <v>1723</v>
       </c>
       <c r="D22" t="s">
         <v>70</v>
@@ -1423,145 +1449,145 @@
         <v>45831</v>
       </c>
       <c r="I22">
-        <v>761.3895</v>
+        <v>761.38940000000002</v>
       </c>
     </row>
     <row r="23" spans="2:11">
       <c r="B23">
-        <v>80001723</v>
+        <v>80001836</v>
       </c>
       <c r="C23">
-        <f>B23-80000000</f>
-        <v>1723</v>
+        <f t="shared" si="0"/>
+        <v>1836</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>156</v>
       </c>
       <c r="F23" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="G23" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="H23">
-        <v>45831</v>
+        <v>98210</v>
       </c>
       <c r="I23">
-        <v>761.38940000000002</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="2:11">
       <c r="B24">
-        <v>80001836</v>
+        <v>80001839</v>
       </c>
       <c r="C24">
-        <f>B24-80000000</f>
-        <v>1836</v>
+        <f t="shared" si="0"/>
+        <v>1839</v>
       </c>
       <c r="D24" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="E24" t="s">
-        <v>156</v>
-      </c>
-      <c r="F24" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="G24" t="s">
-        <v>35</v>
-      </c>
-      <c r="H24">
-        <v>98210</v>
-      </c>
-      <c r="I24">
-        <v>195</v>
+        <v>64</v>
+      </c>
+      <c r="H24" t="s">
+        <v>90</v>
+      </c>
+      <c r="I24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J24">
+        <v>12772</v>
       </c>
     </row>
     <row r="25" spans="2:11">
       <c r="B25">
-        <v>80001839</v>
+        <v>80001840</v>
       </c>
       <c r="C25">
-        <f>B25-80000000</f>
-        <v>1839</v>
+        <f t="shared" si="0"/>
+        <v>1840</v>
       </c>
       <c r="D25" t="s">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>155</v>
+      </c>
+      <c r="F25" t="s">
+        <v>31</v>
       </c>
       <c r="G25" t="s">
-        <v>64</v>
-      </c>
-      <c r="H25" t="s">
-        <v>90</v>
+        <v>2</v>
       </c>
       <c r="I25" t="s">
-        <v>90</v>
-      </c>
-      <c r="J25">
-        <v>12772</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="2:11">
       <c r="B26">
-        <v>80001840</v>
+        <v>80001841</v>
       </c>
       <c r="C26">
-        <f>B26-80000000</f>
-        <v>1840</v>
+        <f t="shared" si="0"/>
+        <v>1841</v>
       </c>
       <c r="D26" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G26" t="s">
-        <v>2</v>
-      </c>
-      <c r="I26" t="s">
-        <v>38</v>
+        <v>9</v>
+      </c>
+      <c r="I26">
+        <v>355.1164</v>
       </c>
     </row>
     <row r="27" spans="2:11">
       <c r="B27">
-        <v>80001841</v>
+        <v>80001842</v>
       </c>
       <c r="C27">
-        <f>B27-80000000</f>
-        <v>1841</v>
+        <f t="shared" si="0"/>
+        <v>1842</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="E27" t="s">
-        <v>153</v>
+        <v>77</v>
       </c>
       <c r="F27" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="G27" t="s">
         <v>9</v>
       </c>
-      <c r="I27">
-        <v>355.1164</v>
+      <c r="H27">
+        <v>87711</v>
+      </c>
+      <c r="I27" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="2:11">
       <c r="B28">
-        <v>80001842</v>
+        <v>80001843</v>
       </c>
       <c r="C28">
-        <f>B28-80000000</f>
-        <v>1842</v>
+        <f t="shared" si="0"/>
+        <v>1843</v>
       </c>
       <c r="D28" t="s">
         <v>70</v>
@@ -1579,124 +1605,124 @@
         <v>87711</v>
       </c>
       <c r="I28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="2:11">
       <c r="B29">
-        <v>80001843</v>
+        <v>80001844</v>
       </c>
       <c r="C29">
-        <f>B29-80000000</f>
-        <v>1843</v>
+        <f t="shared" si="0"/>
+        <v>1844</v>
       </c>
       <c r="D29" t="s">
         <v>70</v>
       </c>
       <c r="E29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F29" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G29" t="s">
         <v>9</v>
       </c>
       <c r="H29">
-        <v>87711</v>
-      </c>
-      <c r="I29" t="s">
-        <v>88</v>
+        <v>313139</v>
+      </c>
+      <c r="I29">
+        <v>765.14480000000003</v>
       </c>
     </row>
     <row r="30" spans="2:11">
       <c r="B30">
-        <v>80001844</v>
+        <v>80001849</v>
       </c>
       <c r="C30">
-        <f>B30-80000000</f>
-        <v>1844</v>
+        <f t="shared" si="0"/>
+        <v>1849</v>
       </c>
       <c r="D30" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="E30" t="s">
-        <v>73</v>
+        <v>154</v>
       </c>
       <c r="F30" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="G30" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30">
-        <v>313139</v>
+        <v>104</v>
       </c>
       <c r="I30">
-        <v>765.14480000000003</v>
+        <v>1128058</v>
+      </c>
+      <c r="K30" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="2:11">
       <c r="B31">
-        <v>80001849</v>
+        <v>80001869</v>
       </c>
       <c r="C31">
-        <f>B31-80000000</f>
-        <v>1849</v>
+        <f t="shared" si="0"/>
+        <v>1869</v>
       </c>
       <c r="D31" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F31" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>104</v>
+        <v>9</v>
+      </c>
+      <c r="H31">
+        <v>77000</v>
       </c>
       <c r="I31">
-        <v>1128058</v>
-      </c>
-      <c r="K31" t="s">
-        <v>112</v>
+        <v>355.12610000000001</v>
       </c>
     </row>
     <row r="32" spans="2:11">
       <c r="B32">
-        <v>80001869</v>
+        <v>80001870</v>
       </c>
       <c r="C32">
-        <f>B32-80000000</f>
-        <v>1869</v>
+        <f t="shared" si="0"/>
+        <v>1870</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="E32" t="s">
-        <v>153</v>
+        <v>77</v>
       </c>
       <c r="F32" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="G32" t="s">
         <v>9</v>
       </c>
       <c r="H32">
-        <v>77000</v>
-      </c>
-      <c r="I32">
-        <v>355.12610000000001</v>
+        <v>87711</v>
+      </c>
+      <c r="I32" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="2:11">
       <c r="B33">
-        <v>80001870</v>
+        <v>80001871</v>
       </c>
       <c r="C33">
-        <f>B33-80000000</f>
-        <v>1870</v>
+        <f t="shared" ref="C33:C64" si="1">B33-80000000</f>
+        <v>1871</v>
       </c>
       <c r="D33" t="s">
         <v>70</v>
@@ -1714,43 +1740,43 @@
         <v>87711</v>
       </c>
       <c r="I33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="2:11">
       <c r="B34">
-        <v>80001871</v>
+        <v>80001872</v>
       </c>
       <c r="C34">
-        <f>B34-80000000</f>
-        <v>1871</v>
+        <f t="shared" si="1"/>
+        <v>1872</v>
       </c>
       <c r="D34" t="s">
         <v>70</v>
       </c>
       <c r="E34" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F34" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G34" t="s">
         <v>9</v>
       </c>
       <c r="H34">
-        <v>87711</v>
-      </c>
-      <c r="I34" t="s">
-        <v>86</v>
+        <v>313139</v>
+      </c>
+      <c r="I34">
+        <v>765.15980000000002</v>
       </c>
     </row>
     <row r="35" spans="2:11">
       <c r="B35">
-        <v>80001872</v>
+        <v>80001873</v>
       </c>
       <c r="C35">
-        <f>B35-80000000</f>
-        <v>1872</v>
+        <f t="shared" si="1"/>
+        <v>1873</v>
       </c>
       <c r="D35" t="s">
         <v>70</v>
@@ -1768,70 +1794,70 @@
         <v>313139</v>
       </c>
       <c r="I35">
-        <v>765.15980000000002</v>
+        <v>765.15970000000004</v>
       </c>
     </row>
     <row r="36" spans="2:11">
       <c r="B36">
-        <v>80001873</v>
+        <v>80001952</v>
       </c>
       <c r="C36">
-        <f>B36-80000000</f>
-        <v>1873</v>
+        <f t="shared" si="1"/>
+        <v>1952</v>
       </c>
       <c r="D36" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="E36" t="s">
-        <v>73</v>
+        <v>154</v>
       </c>
       <c r="F36" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="G36" t="s">
-        <v>9</v>
-      </c>
-      <c r="H36">
-        <v>313139</v>
+        <v>104</v>
       </c>
       <c r="I36">
-        <v>765.15970000000004</v>
+        <v>1173732</v>
+      </c>
+      <c r="K36" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="2:11">
       <c r="B37">
-        <v>80001952</v>
+        <v>80001959</v>
       </c>
       <c r="C37">
-        <f>B37-80000000</f>
-        <v>1952</v>
+        <f t="shared" si="1"/>
+        <v>1959</v>
       </c>
       <c r="D37" t="s">
-        <v>101</v>
+        <v>49</v>
       </c>
       <c r="E37" t="s">
-        <v>154</v>
+        <v>51</v>
       </c>
       <c r="F37" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="G37" t="s">
-        <v>104</v>
+        <v>3</v>
+      </c>
+      <c r="H37" t="s">
+        <v>53</v>
       </c>
       <c r="I37">
-        <v>1173732</v>
-      </c>
-      <c r="K37" t="s">
-        <v>111</v>
+        <v>36193</v>
       </c>
     </row>
     <row r="38" spans="2:11">
       <c r="B38">
-        <v>80001959</v>
+        <v>80001960</v>
       </c>
       <c r="C38">
-        <f>B38-80000000</f>
-        <v>1959</v>
+        <f t="shared" si="1"/>
+        <v>1960</v>
       </c>
       <c r="D38" t="s">
         <v>49</v>
@@ -1849,70 +1875,70 @@
         <v>53</v>
       </c>
       <c r="I38">
-        <v>36193</v>
+        <v>36192</v>
       </c>
     </row>
     <row r="39" spans="2:11">
       <c r="B39">
-        <v>80001960</v>
+        <v>80001965</v>
       </c>
       <c r="C39">
-        <f>B39-80000000</f>
-        <v>1960</v>
+        <f t="shared" si="1"/>
+        <v>1965</v>
       </c>
       <c r="D39" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="E39" t="s">
-        <v>51</v>
+        <v>153</v>
       </c>
       <c r="F39" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>3</v>
-      </c>
-      <c r="H39" t="s">
-        <v>53</v>
+        <v>9</v>
+      </c>
+      <c r="H39">
+        <v>77000</v>
       </c>
       <c r="I39">
-        <v>36192</v>
+        <v>355.1354</v>
       </c>
     </row>
     <row r="40" spans="2:11">
       <c r="B40">
-        <v>80001965</v>
+        <v>80001996</v>
       </c>
       <c r="C40">
-        <f>B40-80000000</f>
-        <v>1965</v>
+        <f t="shared" si="1"/>
+        <v>1996</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="E40" t="s">
-        <v>153</v>
+        <v>77</v>
       </c>
       <c r="F40" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="G40" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H40">
-        <v>77000</v>
+        <v>87711</v>
       </c>
       <c r="I40">
-        <v>355.1354</v>
+        <v>722.21799999999996</v>
       </c>
     </row>
     <row r="41" spans="2:11">
       <c r="B41">
-        <v>80001996</v>
+        <v>80001997</v>
       </c>
       <c r="C41">
-        <f>B41-80000000</f>
-        <v>1996</v>
+        <f t="shared" si="1"/>
+        <v>1997</v>
       </c>
       <c r="D41" t="s">
         <v>70</v>
@@ -1930,193 +1956,199 @@
         <v>87711</v>
       </c>
       <c r="I41">
-        <v>722.21799999999996</v>
+        <v>722.21810000000005</v>
       </c>
     </row>
     <row r="42" spans="2:11">
       <c r="B42">
-        <v>80001997</v>
+        <v>80002000</v>
       </c>
       <c r="C42">
-        <f>B42-80000000</f>
-        <v>1997</v>
+        <f t="shared" si="1"/>
+        <v>2000</v>
       </c>
       <c r="D42" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="E42" t="s">
-        <v>77</v>
+        <v>154</v>
       </c>
       <c r="F42" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="G42" t="s">
-        <v>2</v>
-      </c>
-      <c r="H42">
-        <v>87711</v>
+        <v>104</v>
       </c>
       <c r="I42">
-        <v>722.21810000000005</v>
+        <v>1184166</v>
+      </c>
+      <c r="K42" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="2:11">
       <c r="B43">
-        <v>80002000</v>
+        <v>80002009</v>
       </c>
       <c r="C43">
-        <f>B43-80000000</f>
-        <v>2000</v>
+        <f t="shared" si="1"/>
+        <v>2009</v>
       </c>
       <c r="D43" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="E43" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="F43" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="G43" t="s">
-        <v>104</v>
-      </c>
-      <c r="I43">
-        <v>1184166</v>
+        <v>124</v>
+      </c>
+      <c r="I43" t="s">
+        <v>125</v>
       </c>
       <c r="K43" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="2:11">
       <c r="B44">
-        <v>80002009</v>
+        <v>80002036</v>
       </c>
       <c r="C44">
-        <f>B44-80000000</f>
-        <v>2009</v>
+        <f t="shared" si="1"/>
+        <v>2036</v>
       </c>
       <c r="D44" t="s">
-        <v>117</v>
+        <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="F44" t="s">
-        <v>123</v>
+        <v>31</v>
       </c>
       <c r="G44" t="s">
-        <v>124</v>
-      </c>
-      <c r="I44" t="s">
-        <v>125</v>
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>89000</v>
+      </c>
+      <c r="I44">
+        <v>177</v>
+      </c>
+      <c r="J44">
+        <v>12991</v>
       </c>
       <c r="K44" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="2:11">
       <c r="B45">
-        <v>80002036</v>
+        <v>80002073</v>
       </c>
       <c r="C45">
-        <f>B45-80000000</f>
-        <v>2036</v>
+        <f t="shared" si="1"/>
+        <v>2073</v>
       </c>
       <c r="D45" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="E45" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F45" t="s">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="G45" t="s">
-        <v>2</v>
-      </c>
-      <c r="H45">
-        <v>89000</v>
+        <v>104</v>
       </c>
       <c r="I45">
-        <v>177</v>
+        <v>1190766</v>
       </c>
       <c r="J45">
-        <v>12991</v>
+        <v>13002</v>
       </c>
       <c r="K45" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="2:11">
       <c r="B46">
-        <v>80002073</v>
+        <v>80002099</v>
       </c>
       <c r="C46">
-        <f>B46-80000000</f>
-        <v>2073</v>
+        <f t="shared" si="1"/>
+        <v>2099</v>
       </c>
       <c r="D46" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="E46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F46" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="G46" t="s">
-        <v>104</v>
+        <v>9</v>
+      </c>
+      <c r="H46">
+        <v>77000</v>
       </c>
       <c r="I46">
-        <v>1190766</v>
+        <v>355.14589999999998</v>
       </c>
       <c r="J46">
-        <v>13002</v>
+        <v>13033</v>
       </c>
       <c r="K46" t="s">
-        <v>109</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="2:11">
       <c r="B47">
-        <v>80002099</v>
+        <v>80002100</v>
       </c>
       <c r="C47">
-        <f>B47-80000000</f>
-        <v>2099</v>
+        <f t="shared" si="1"/>
+        <v>2100</v>
       </c>
       <c r="D47" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="E47" t="s">
-        <v>153</v>
+        <v>77</v>
       </c>
       <c r="F47" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="G47" t="s">
         <v>9</v>
       </c>
       <c r="H47">
-        <v>77000</v>
+        <v>87711</v>
       </c>
       <c r="I47">
-        <v>355.14589999999998</v>
+        <v>2293</v>
       </c>
       <c r="J47">
-        <v>13033</v>
+        <v>13034</v>
       </c>
       <c r="K47" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="2:11">
       <c r="B48">
-        <v>80002100</v>
+        <v>80002101</v>
       </c>
       <c r="C48">
-        <f>B48-80000000</f>
-        <v>2100</v>
+        <f t="shared" si="1"/>
+        <v>2101</v>
       </c>
       <c r="D48" t="s">
         <v>70</v>
@@ -2134,82 +2166,79 @@
         <v>87711</v>
       </c>
       <c r="I48">
-        <v>2293</v>
+        <v>2292</v>
       </c>
       <c r="J48">
-        <v>13034</v>
+        <v>13035</v>
       </c>
       <c r="K48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="2:11">
       <c r="B49">
-        <v>80002101</v>
+        <v>80002114</v>
       </c>
       <c r="C49">
-        <f>B49-80000000</f>
-        <v>2101</v>
+        <f t="shared" si="1"/>
+        <v>2114</v>
       </c>
       <c r="D49" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="E49" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="F49" t="s">
-        <v>78</v>
+        <v>119</v>
       </c>
       <c r="G49" t="s">
-        <v>9</v>
-      </c>
-      <c r="H49">
-        <v>87711</v>
+        <v>120</v>
       </c>
       <c r="I49">
-        <v>2292</v>
-      </c>
-      <c r="J49">
-        <v>13035</v>
+        <v>310130</v>
       </c>
       <c r="K49" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="2:11">
       <c r="B50">
-        <v>80002114</v>
+        <v>80002147</v>
       </c>
       <c r="C50">
-        <f>B50-80000000</f>
-        <v>2114</v>
+        <f t="shared" si="1"/>
+        <v>2147</v>
       </c>
       <c r="D50" t="s">
-        <v>117</v>
+        <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>118</v>
+        <v>156</v>
       </c>
       <c r="F50" t="s">
-        <v>119</v>
+        <v>34</v>
       </c>
       <c r="G50" t="s">
-        <v>120</v>
+        <v>35</v>
       </c>
       <c r="I50">
-        <v>310130</v>
+        <v>280</v>
+      </c>
+      <c r="J50">
+        <v>13088</v>
       </c>
       <c r="K50" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="2:11">
       <c r="B51">
-        <v>80002147</v>
+        <v>80002148</v>
       </c>
       <c r="C51">
-        <f>B51-80000000</f>
-        <v>2147</v>
+        <f t="shared" si="1"/>
+        <v>2148</v>
       </c>
       <c r="D51" t="s">
         <v>0</v>
@@ -2224,97 +2253,94 @@
         <v>35</v>
       </c>
       <c r="I51">
-        <v>280</v>
-      </c>
-      <c r="J51">
-        <v>13088</v>
-      </c>
-      <c r="K51" t="s">
-        <v>37</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="2:11">
       <c r="B52">
-        <v>80002148</v>
+        <v>80002223</v>
       </c>
       <c r="C52">
-        <f>B52-80000000</f>
-        <v>2148</v>
+        <f t="shared" si="1"/>
+        <v>2223</v>
       </c>
       <c r="D52" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E52" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="F52" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="G52" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="I52">
-        <v>281</v>
+        <v>50385</v>
       </c>
     </row>
     <row r="53" spans="2:11">
       <c r="B53">
-        <v>80002223</v>
+        <v>80002255</v>
       </c>
       <c r="C53">
-        <f>B53-80000000</f>
-        <v>2223</v>
+        <f t="shared" si="1"/>
+        <v>2255</v>
       </c>
       <c r="D53" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E53" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="F53" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G53" t="s">
-        <v>20</v>
+        <v>9</v>
+      </c>
+      <c r="H53">
+        <v>77000</v>
       </c>
       <c r="I53">
-        <v>50385</v>
+        <v>355.15559999999999</v>
       </c>
     </row>
     <row r="54" spans="2:11">
       <c r="B54">
-        <v>80002255</v>
+        <v>80002256</v>
       </c>
       <c r="C54">
-        <f>B54-80000000</f>
-        <v>2255</v>
+        <f t="shared" si="1"/>
+        <v>2256</v>
       </c>
       <c r="D54" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="E54" t="s">
-        <v>153</v>
+        <v>77</v>
       </c>
       <c r="F54" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="G54" t="s">
         <v>9</v>
       </c>
       <c r="H54">
-        <v>77000</v>
+        <v>87711</v>
       </c>
       <c r="I54">
-        <v>355.15559999999999</v>
+        <v>2456</v>
       </c>
     </row>
     <row r="55" spans="2:11">
       <c r="B55">
-        <v>80002256</v>
+        <v>80002257</v>
       </c>
       <c r="C55">
-        <f>B55-80000000</f>
-        <v>2256</v>
+        <f t="shared" si="1"/>
+        <v>2257</v>
       </c>
       <c r="D55" t="s">
         <v>70</v>
@@ -2332,133 +2358,136 @@
         <v>87711</v>
       </c>
       <c r="I55">
-        <v>2456</v>
+        <v>2457</v>
       </c>
     </row>
     <row r="56" spans="2:11">
       <c r="B56">
-        <v>80002257</v>
+        <v>80002258</v>
       </c>
       <c r="C56">
-        <f>B56-80000000</f>
-        <v>2257</v>
+        <f t="shared" si="1"/>
+        <v>2258</v>
       </c>
       <c r="D56" t="s">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>77</v>
+        <v>155</v>
       </c>
       <c r="F56" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="G56" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H56">
-        <v>87711</v>
+        <v>89000</v>
       </c>
       <c r="I56">
-        <v>2457</v>
+        <v>202</v>
       </c>
     </row>
     <row r="57" spans="2:11">
       <c r="B57">
-        <v>80002258</v>
+        <v>80002264</v>
       </c>
       <c r="C57">
-        <f>B57-80000000</f>
-        <v>2258</v>
+        <f t="shared" si="1"/>
+        <v>2264</v>
       </c>
       <c r="D57" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="E57" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F57" t="s">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="G57" t="s">
-        <v>2</v>
-      </c>
-      <c r="H57">
-        <v>89000</v>
+        <v>104</v>
       </c>
       <c r="I57">
-        <v>202</v>
+        <v>1219638</v>
+      </c>
+      <c r="J57">
+        <v>13186</v>
+      </c>
+      <c r="K57" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="2:11">
       <c r="B58">
-        <v>80002264</v>
+        <v>80002290</v>
       </c>
       <c r="C58">
-        <f>B58-80000000</f>
-        <v>2264</v>
+        <f t="shared" si="1"/>
+        <v>2290</v>
       </c>
       <c r="D58" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="E58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F58" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="G58" t="s">
-        <v>104</v>
+        <v>9</v>
+      </c>
+      <c r="H58">
+        <v>77000</v>
       </c>
       <c r="I58">
-        <v>1219638</v>
+        <v>355.16120000000001</v>
       </c>
       <c r="J58">
-        <v>13186</v>
+        <v>13207</v>
       </c>
       <c r="K58" t="s">
-        <v>108</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59" spans="2:11">
       <c r="B59">
-        <v>80002290</v>
+        <v>80002291</v>
       </c>
       <c r="C59">
-        <f>B59-80000000</f>
-        <v>2290</v>
+        <f t="shared" si="1"/>
+        <v>2291</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="E59" t="s">
-        <v>153</v>
+        <v>77</v>
       </c>
       <c r="F59" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="G59" t="s">
         <v>9</v>
       </c>
       <c r="H59">
-        <v>77000</v>
+        <v>87711</v>
       </c>
       <c r="I59">
-        <v>355.16120000000001</v>
-      </c>
-      <c r="J59">
-        <v>13207</v>
+        <v>2548</v>
       </c>
       <c r="K59" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" spans="2:11">
       <c r="B60">
-        <v>80002291</v>
+        <v>80002292</v>
       </c>
       <c r="C60">
-        <f>B60-80000000</f>
-        <v>2291</v>
+        <f t="shared" si="1"/>
+        <v>2292</v>
       </c>
       <c r="D60" t="s">
         <v>70</v>
@@ -2476,148 +2505,151 @@
         <v>87711</v>
       </c>
       <c r="I60">
-        <v>2548</v>
+        <v>2549</v>
+      </c>
+      <c r="J60">
+        <v>13209</v>
       </c>
       <c r="K60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="2:11">
       <c r="B61">
-        <v>80002292</v>
+        <v>80002293</v>
       </c>
       <c r="C61">
-        <f>B61-80000000</f>
-        <v>2292</v>
+        <f t="shared" si="1"/>
+        <v>2293</v>
       </c>
       <c r="D61" t="s">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>77</v>
+        <v>155</v>
       </c>
       <c r="F61" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="G61" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H61">
-        <v>87711</v>
+        <v>89000</v>
       </c>
       <c r="I61">
-        <v>2549</v>
+        <v>188.02109999999999</v>
       </c>
       <c r="J61">
-        <v>13209</v>
+        <v>13206</v>
       </c>
       <c r="K61" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="2:11">
       <c r="B62">
-        <v>80002293</v>
+        <v>80002351</v>
       </c>
       <c r="C62">
-        <f>B62-80000000</f>
-        <v>2293</v>
+        <f t="shared" si="1"/>
+        <v>2351</v>
       </c>
       <c r="D62" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="E62" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F62" t="s">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="G62" t="s">
-        <v>2</v>
-      </c>
-      <c r="H62">
-        <v>89000</v>
+        <v>104</v>
       </c>
       <c r="I62">
-        <v>188.02109999999999</v>
+        <v>10588026</v>
       </c>
       <c r="J62">
-        <v>13206</v>
+        <v>13235</v>
       </c>
       <c r="K62" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
     </row>
     <row r="63" spans="2:11">
       <c r="B63">
-        <v>80002351</v>
+        <v>80002352</v>
       </c>
       <c r="C63">
-        <f>B63-80000000</f>
-        <v>2351</v>
+        <f t="shared" si="1"/>
+        <v>2352</v>
       </c>
       <c r="D63" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="E63" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F63" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="G63" t="s">
-        <v>104</v>
+        <v>9</v>
+      </c>
+      <c r="H63">
+        <v>77000</v>
       </c>
       <c r="I63">
-        <v>10588026</v>
+        <v>355.16899999999998</v>
       </c>
       <c r="J63">
-        <v>13235</v>
+        <v>13237</v>
       </c>
       <c r="K63" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="2:11">
       <c r="B64">
-        <v>80002352</v>
+        <v>80002353</v>
       </c>
       <c r="C64">
-        <f>B64-80000000</f>
-        <v>2352</v>
+        <f t="shared" si="1"/>
+        <v>2353</v>
       </c>
       <c r="D64" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="E64" t="s">
-        <v>153</v>
+        <v>77</v>
       </c>
       <c r="F64" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="G64" t="s">
         <v>9</v>
       </c>
       <c r="H64">
-        <v>77000</v>
+        <v>87711</v>
       </c>
       <c r="I64">
-        <v>355.16899999999998</v>
+        <v>2667</v>
       </c>
       <c r="J64">
-        <v>13237</v>
+        <v>13238</v>
       </c>
       <c r="K64" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
     </row>
     <row r="65" spans="2:11">
       <c r="B65">
-        <v>80002353</v>
+        <v>80002354</v>
       </c>
       <c r="C65">
-        <f>B65-80000000</f>
-        <v>2353</v>
+        <f t="shared" ref="C65:C93" si="2">B65-80000000</f>
+        <v>2354</v>
       </c>
       <c r="D65" t="s">
         <v>70</v>
@@ -2635,109 +2667,103 @@
         <v>87711</v>
       </c>
       <c r="I65">
-        <v>2667</v>
+        <v>2668</v>
       </c>
       <c r="J65">
-        <v>13238</v>
+        <v>13239</v>
       </c>
       <c r="K65" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="2:11">
       <c r="B66">
-        <v>80002354</v>
+        <v>80002458</v>
       </c>
       <c r="C66">
-        <f>B66-80000000</f>
-        <v>2354</v>
+        <f t="shared" si="2"/>
+        <v>2458</v>
       </c>
       <c r="D66" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="E66" t="s">
-        <v>77</v>
+        <v>158</v>
       </c>
       <c r="F66" t="s">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="G66" t="s">
         <v>9</v>
       </c>
-      <c r="H66">
-        <v>87711</v>
-      </c>
       <c r="I66">
-        <v>2668</v>
-      </c>
-      <c r="J66">
-        <v>13239</v>
-      </c>
-      <c r="K66" t="s">
-        <v>79</v>
+        <v>333.28440000000001</v>
       </c>
     </row>
     <row r="67" spans="2:11">
       <c r="B67">
-        <v>80002458</v>
+        <v>80002467</v>
       </c>
       <c r="C67">
-        <f>B67-80000000</f>
-        <v>2458</v>
+        <f t="shared" si="2"/>
+        <v>2467</v>
       </c>
       <c r="D67" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="E67" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F67" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="G67" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="I67">
-        <v>333.28440000000001</v>
+        <v>10588026</v>
+      </c>
+      <c r="J67">
+        <v>13268</v>
+      </c>
+      <c r="K67" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="68" spans="2:11">
       <c r="B68">
-        <v>80002467</v>
+        <v>80002469</v>
       </c>
       <c r="C68">
-        <f>B68-80000000</f>
-        <v>2467</v>
+        <f t="shared" si="2"/>
+        <v>2469</v>
       </c>
       <c r="D68" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="E68" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F68" t="s">
-        <v>103</v>
+        <v>31</v>
       </c>
       <c r="G68" t="s">
-        <v>104</v>
-      </c>
-      <c r="I68">
-        <v>10588026</v>
-      </c>
-      <c r="J68">
-        <v>13268</v>
-      </c>
-      <c r="K68" t="s">
-        <v>106</v>
+        <v>2</v>
+      </c>
+      <c r="H68">
+        <v>89000</v>
+      </c>
+      <c r="I68" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="69" spans="2:11">
       <c r="B69">
-        <v>80002469</v>
+        <v>80002475</v>
       </c>
       <c r="C69">
-        <f>B69-80000000</f>
-        <v>2469</v>
+        <f t="shared" si="2"/>
+        <v>2475</v>
       </c>
       <c r="D69" t="s">
         <v>0</v>
@@ -2746,52 +2772,52 @@
         <v>155</v>
       </c>
       <c r="F69" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="G69" t="s">
         <v>2</v>
       </c>
       <c r="H69">
-        <v>89000</v>
-      </c>
-      <c r="I69" t="s">
-        <v>32</v>
+        <v>58000</v>
+      </c>
+      <c r="I69">
+        <v>188.011</v>
       </c>
     </row>
     <row r="70" spans="2:11">
       <c r="B70">
-        <v>80002475</v>
+        <v>80002483</v>
       </c>
       <c r="C70">
-        <f>B70-80000000</f>
-        <v>2475</v>
+        <f t="shared" si="2"/>
+        <v>2483</v>
       </c>
       <c r="D70" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="E70" t="s">
-        <v>155</v>
+        <v>77</v>
       </c>
       <c r="F70" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="G70" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H70">
-        <v>58000</v>
+        <v>60938</v>
       </c>
       <c r="I70">
-        <v>188.011</v>
+        <v>721.19680000000005</v>
       </c>
     </row>
     <row r="71" spans="2:11">
       <c r="B71">
-        <v>80002483</v>
+        <v>80002484</v>
       </c>
       <c r="C71">
-        <f>B71-80000000</f>
-        <v>2483</v>
+        <f t="shared" si="2"/>
+        <v>2484</v>
       </c>
       <c r="D71" t="s">
         <v>70</v>
@@ -2809,16 +2835,16 @@
         <v>60938</v>
       </c>
       <c r="I71">
-        <v>721.19680000000005</v>
+        <v>721.23140000000001</v>
       </c>
     </row>
     <row r="72" spans="2:11">
       <c r="B72">
-        <v>80002484</v>
+        <v>80002485</v>
       </c>
       <c r="C72">
-        <f>B72-80000000</f>
-        <v>2484</v>
+        <f t="shared" si="2"/>
+        <v>2485</v>
       </c>
       <c r="D72" t="s">
         <v>70</v>
@@ -2836,238 +2862,244 @@
         <v>60938</v>
       </c>
       <c r="I72">
-        <v>721.23140000000001</v>
+        <v>721.23130000000003</v>
       </c>
     </row>
     <row r="73" spans="2:11">
       <c r="B73">
-        <v>80002485</v>
+        <v>80002486</v>
       </c>
       <c r="C73">
-        <f>B73-80000000</f>
-        <v>2485</v>
+        <f t="shared" si="2"/>
+        <v>2486</v>
       </c>
       <c r="D73" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="E73" t="s">
-        <v>77</v>
+        <v>157</v>
       </c>
       <c r="F73" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="G73" t="s">
-        <v>9</v>
-      </c>
-      <c r="H73">
-        <v>60938</v>
+        <v>3</v>
+      </c>
+      <c r="H73" t="s">
+        <v>53</v>
       </c>
       <c r="I73">
-        <v>721.23130000000003</v>
+        <v>36191</v>
       </c>
     </row>
     <row r="74" spans="2:11">
       <c r="B74">
-        <v>80002486</v>
+        <v>80002492</v>
       </c>
       <c r="C74">
-        <f>B74-80000000</f>
-        <v>2486</v>
+        <f t="shared" si="2"/>
+        <v>2492</v>
       </c>
       <c r="D74" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="E74" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F74" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
       <c r="G74" t="s">
-        <v>3</v>
-      </c>
-      <c r="H74" t="s">
-        <v>53</v>
-      </c>
-      <c r="I74">
-        <v>36191</v>
+        <v>104</v>
+      </c>
+      <c r="I74" t="s">
+        <v>105</v>
+      </c>
+      <c r="K74" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="2:11">
       <c r="B75">
-        <v>80002492</v>
+        <v>80002647</v>
       </c>
       <c r="C75">
-        <f>B75-80000000</f>
-        <v>2492</v>
+        <f t="shared" si="2"/>
+        <v>2647</v>
       </c>
       <c r="D75" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="E75" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="F75" t="s">
-        <v>103</v>
+        <v>136</v>
       </c>
       <c r="G75" t="s">
-        <v>104</v>
+        <v>99</v>
+      </c>
+      <c r="H75" t="s">
+        <v>139</v>
       </c>
       <c r="I75" t="s">
-        <v>105</v>
-      </c>
-      <c r="K75" t="s">
-        <v>5</v>
+        <v>140</v>
       </c>
     </row>
     <row r="76" spans="2:11">
       <c r="B76">
-        <v>80002647</v>
+        <v>80002685</v>
       </c>
       <c r="C76">
-        <f>B76-80000000</f>
-        <v>2647</v>
+        <f t="shared" si="2"/>
+        <v>2685</v>
       </c>
       <c r="D76" t="s">
-        <v>134</v>
+        <v>7</v>
       </c>
       <c r="E76" t="s">
-        <v>135</v>
+        <v>10</v>
       </c>
       <c r="F76" t="s">
-        <v>136</v>
+        <v>11</v>
       </c>
       <c r="G76" t="s">
-        <v>99</v>
-      </c>
-      <c r="H76" t="s">
-        <v>139</v>
-      </c>
-      <c r="I76" t="s">
-        <v>140</v>
+        <v>9</v>
+      </c>
+      <c r="H76">
+        <v>77777</v>
+      </c>
+      <c r="I76">
+        <v>320.04050000000001</v>
+      </c>
+      <c r="J76">
+        <v>13382</v>
       </c>
     </row>
     <row r="77" spans="2:11">
       <c r="B77">
-        <v>80002685</v>
+        <v>80002686</v>
       </c>
       <c r="C77">
-        <f>B77-80000000</f>
-        <v>2685</v>
+        <f t="shared" si="2"/>
+        <v>2686</v>
       </c>
       <c r="D77" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="E77" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="F77" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="G77" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H77">
-        <v>77777</v>
+        <v>82999</v>
       </c>
       <c r="I77">
-        <v>320.04050000000001</v>
+        <v>119.0064</v>
       </c>
       <c r="J77">
-        <v>13382</v>
+        <v>13383</v>
       </c>
     </row>
     <row r="78" spans="2:11">
       <c r="B78">
-        <v>80002686</v>
+        <v>80002691</v>
       </c>
       <c r="C78">
-        <f>B78-80000000</f>
-        <v>2686</v>
+        <f t="shared" si="2"/>
+        <v>2691</v>
       </c>
       <c r="D78" t="s">
-        <v>70</v>
+        <v>134</v>
       </c>
       <c r="E78" t="s">
-        <v>74</v>
+        <v>135</v>
       </c>
       <c r="F78" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="G78" t="s">
-        <v>2</v>
-      </c>
-      <c r="H78">
-        <v>82999</v>
-      </c>
-      <c r="I78">
-        <v>119.0064</v>
-      </c>
-      <c r="J78">
-        <v>13383</v>
+        <v>99</v>
+      </c>
+      <c r="H78" t="s">
+        <v>137</v>
+      </c>
+      <c r="I78" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="79" spans="2:11">
       <c r="B79">
-        <v>80002691</v>
+        <v>80002715</v>
       </c>
       <c r="C79">
-        <f>B79-80000000</f>
-        <v>2691</v>
+        <f t="shared" si="2"/>
+        <v>2715</v>
       </c>
       <c r="D79" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="E79" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="F79" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="G79" t="s">
-        <v>99</v>
-      </c>
-      <c r="H79" t="s">
-        <v>137</v>
-      </c>
-      <c r="I79" t="s">
-        <v>138</v>
+        <v>104</v>
+      </c>
+      <c r="I79">
+        <v>1352440</v>
+      </c>
+      <c r="K79" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="2:11">
       <c r="B80">
-        <v>80002715</v>
+        <v>80002716</v>
       </c>
       <c r="C80">
-        <f>B80-80000000</f>
-        <v>2715</v>
+        <f t="shared" si="2"/>
+        <v>2716</v>
       </c>
       <c r="D80" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F80" t="s">
-        <v>103</v>
+        <v>26</v>
       </c>
       <c r="G80" t="s">
-        <v>104</v>
+        <v>27</v>
+      </c>
+      <c r="H80">
+        <v>1941317</v>
       </c>
       <c r="I80">
-        <v>1352440</v>
+        <v>928</v>
+      </c>
+      <c r="J80">
+        <v>13407</v>
       </c>
       <c r="K80" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="81" spans="2:11">
       <c r="B81">
-        <v>80002716</v>
+        <v>80002717</v>
       </c>
       <c r="C81">
-        <f>B81-80000000</f>
-        <v>2716</v>
+        <f t="shared" si="2"/>
+        <v>2717</v>
       </c>
       <c r="D81" t="s">
         <v>0</v>
@@ -3085,55 +3117,49 @@
         <v>1941317</v>
       </c>
       <c r="I81">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="J81">
-        <v>13407</v>
+        <v>13408</v>
       </c>
       <c r="K81" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="82" spans="2:11">
       <c r="B82">
-        <v>80002717</v>
+        <v>80002783</v>
       </c>
       <c r="C82">
-        <f>B82-80000000</f>
-        <v>2717</v>
+        <f t="shared" si="2"/>
+        <v>2783</v>
       </c>
       <c r="D82" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="E82" t="s">
-        <v>156</v>
+        <v>73</v>
       </c>
       <c r="F82" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="G82" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="H82">
-        <v>1941317</v>
+        <v>313139</v>
       </c>
       <c r="I82">
-        <v>929</v>
-      </c>
-      <c r="J82">
-        <v>13408</v>
-      </c>
-      <c r="K82" t="s">
-        <v>28</v>
+        <v>765.26089999999999</v>
       </c>
     </row>
     <row r="83" spans="2:11">
       <c r="B83">
-        <v>80002783</v>
+        <v>80002784</v>
       </c>
       <c r="C83">
-        <f>B83-80000000</f>
-        <v>2783</v>
+        <f t="shared" si="2"/>
+        <v>2784</v>
       </c>
       <c r="D83" t="s">
         <v>70</v>
@@ -3151,100 +3177,103 @@
         <v>313139</v>
       </c>
       <c r="I83">
-        <v>765.26089999999999</v>
+        <v>765.26099999999997</v>
       </c>
     </row>
     <row r="84" spans="2:11">
       <c r="B84">
-        <v>80002784</v>
+        <v>80002860</v>
       </c>
       <c r="C84">
-        <f>B84-80000000</f>
-        <v>2784</v>
+        <f t="shared" si="2"/>
+        <v>2860</v>
       </c>
       <c r="D84" t="s">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="E84" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="F84" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="G84" t="s">
-        <v>9</v>
-      </c>
-      <c r="H84">
-        <v>313139</v>
+        <v>23</v>
+      </c>
+      <c r="H84" t="s">
+        <v>24</v>
       </c>
       <c r="I84">
-        <v>765.26099999999997</v>
+        <v>10621</v>
       </c>
     </row>
     <row r="85" spans="2:11">
       <c r="B85">
-        <v>80002860</v>
+        <v>80002903</v>
       </c>
       <c r="C85">
-        <f>B85-80000000</f>
-        <v>2860</v>
+        <f t="shared" si="2"/>
+        <v>2903</v>
       </c>
       <c r="D85" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E85" t="s">
-        <v>21</v>
+        <v>153</v>
       </c>
       <c r="F85" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="G85" t="s">
-        <v>23</v>
-      </c>
-      <c r="H85" t="s">
-        <v>24</v>
+        <v>9</v>
+      </c>
+      <c r="H85">
+        <v>318000</v>
       </c>
       <c r="I85">
-        <v>10621</v>
+        <v>355.22059999999999</v>
+      </c>
+      <c r="J85">
+        <v>13578</v>
       </c>
     </row>
     <row r="86" spans="2:11">
       <c r="B86">
-        <v>80002903</v>
+        <v>80002904</v>
       </c>
       <c r="C86">
-        <f>B86-80000000</f>
-        <v>2903</v>
+        <f t="shared" si="2"/>
+        <v>2904</v>
       </c>
       <c r="D86" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="E86" t="s">
-        <v>153</v>
+        <v>77</v>
       </c>
       <c r="F86" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="G86" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H86">
-        <v>318000</v>
+        <v>76847</v>
       </c>
       <c r="I86">
-        <v>355.22059999999999</v>
+        <v>722.26959999999997</v>
       </c>
       <c r="J86">
-        <v>13578</v>
+        <v>13579</v>
       </c>
     </row>
     <row r="87" spans="2:11">
       <c r="B87">
-        <v>80002904</v>
+        <v>80002905</v>
       </c>
       <c r="C87">
-        <f>B87-80000000</f>
-        <v>2904</v>
+        <f t="shared" si="2"/>
+        <v>2905</v>
       </c>
       <c r="D87" t="s">
         <v>70</v>
@@ -3262,49 +3291,49 @@
         <v>76847</v>
       </c>
       <c r="I87">
-        <v>722.26959999999997</v>
+        <v>722.26969999999994</v>
       </c>
       <c r="J87">
-        <v>13579</v>
+        <v>13580</v>
       </c>
     </row>
     <row r="88" spans="2:11">
       <c r="B88">
-        <v>80002905</v>
+        <v>80002906</v>
       </c>
       <c r="C88">
-        <f>B88-80000000</f>
-        <v>2905</v>
+        <f t="shared" si="2"/>
+        <v>2906</v>
       </c>
       <c r="D88" t="s">
         <v>70</v>
       </c>
       <c r="E88" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F88" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G88" t="s">
         <v>2</v>
       </c>
       <c r="H88">
-        <v>76847</v>
+        <v>313139</v>
       </c>
       <c r="I88">
-        <v>722.26969999999994</v>
+        <v>765.28880000000004</v>
       </c>
       <c r="J88">
-        <v>13580</v>
+        <v>13581</v>
       </c>
     </row>
     <row r="89" spans="2:11">
       <c r="B89">
-        <v>80002906</v>
+        <v>80002907</v>
       </c>
       <c r="C89">
-        <f>B89-80000000</f>
-        <v>2906</v>
+        <f t="shared" si="2"/>
+        <v>2907</v>
       </c>
       <c r="D89" t="s">
         <v>70</v>
@@ -3322,103 +3351,97 @@
         <v>313139</v>
       </c>
       <c r="I89">
-        <v>765.28880000000004</v>
+        <v>765.29290000000003</v>
       </c>
       <c r="J89">
-        <v>13581</v>
+        <v>13582</v>
       </c>
     </row>
     <row r="90" spans="2:11">
       <c r="B90">
-        <v>80002907</v>
+        <v>80002934</v>
       </c>
       <c r="C90">
-        <f>B90-80000000</f>
-        <v>2907</v>
+        <f t="shared" si="2"/>
+        <v>2934</v>
       </c>
       <c r="D90" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="E90" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="F90" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="G90" t="s">
-        <v>2</v>
-      </c>
-      <c r="H90">
-        <v>313139</v>
-      </c>
-      <c r="I90">
-        <v>765.29290000000003</v>
-      </c>
-      <c r="J90">
-        <v>13582</v>
+        <v>99</v>
+      </c>
+      <c r="I90" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="2:11">
       <c r="B91">
-        <v>80002934</v>
+        <v>80003383</v>
       </c>
       <c r="C91">
-        <f>B91-80000000</f>
-        <v>2934</v>
+        <f t="shared" si="2"/>
+        <v>3383</v>
       </c>
       <c r="D91" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E91" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="F91" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="G91" t="s">
-        <v>99</v>
-      </c>
-      <c r="I91" t="s">
-        <v>100</v>
+        <v>104</v>
+      </c>
+      <c r="H91">
+        <v>10664849</v>
+      </c>
+      <c r="I91">
+        <v>1629931</v>
+      </c>
+      <c r="K91" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="2:11">
       <c r="B92">
-        <v>80003383</v>
+        <v>80003384</v>
       </c>
       <c r="C92">
-        <f>B92-80000000</f>
-        <v>3383</v>
+        <f t="shared" si="2"/>
+        <v>3384</v>
       </c>
       <c r="D92" t="s">
-        <v>101</v>
+        <v>49</v>
       </c>
       <c r="E92" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="F92" t="s">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="G92" t="s">
-        <v>104</v>
-      </c>
-      <c r="H92">
-        <v>10664849</v>
+        <v>3</v>
       </c>
       <c r="I92">
-        <v>1629931</v>
-      </c>
-      <c r="K92" t="s">
-        <v>5</v>
+        <v>60644</v>
       </c>
     </row>
     <row r="93" spans="2:11">
       <c r="B93">
-        <v>80003384</v>
+        <v>80003385</v>
       </c>
       <c r="C93">
-        <f>B93-80000000</f>
-        <v>3384</v>
+        <f t="shared" si="2"/>
+        <v>3385</v>
       </c>
       <c r="D93" t="s">
         <v>49</v>
@@ -3433,39 +3456,10 @@
         <v>3</v>
       </c>
       <c r="I93">
-        <v>60644</v>
-      </c>
-    </row>
-    <row r="94" spans="2:11">
-      <c r="B94">
-        <v>80003385</v>
-      </c>
-      <c r="C94">
-        <f>B94-80000000</f>
-        <v>3385</v>
-      </c>
-      <c r="D94" t="s">
-        <v>49</v>
-      </c>
-      <c r="E94" t="s">
-        <v>157</v>
-      </c>
-      <c r="F94" t="s">
-        <v>50</v>
-      </c>
-      <c r="G94" t="s">
-        <v>3</v>
-      </c>
-      <c r="I94">
         <v>60643</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K94">
-    <sortState ref="B2:U93">
-      <sortCondition ref="C1:C93"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>